<commit_message>
Weighting & Scaling update & heatmap
</commit_message>
<xml_diff>
--- a/data/input/preprocessing/ecology/ecology_values_PLA_Cuboid.xlsx
+++ b/data/input/preprocessing/ecology/ecology_values_PLA_Cuboid.xlsx
@@ -1,23 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/test_inputs/preprocessing/ecology_format/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/input/preprocessing/ecology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC6C0D4-80D2-A04A-BFF5-F01693F54E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4998256C-B0FF-4A4B-9F6A-18FEF5AEE1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13860" yWindow="500" windowWidth="17680" windowHeight="16780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33620" yWindow="500" windowWidth="19080" windowHeight="21100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ecological_params" sheetId="1" r:id="rId1"/>
     <sheet name="Scaling" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -26,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Alternative_Param</t>
   </si>
@@ -56,6 +66,12 @@
   </si>
   <si>
     <t>PLA_recycled_industrial</t>
+  </si>
+  <si>
+    <t>Optimal</t>
+  </si>
+  <si>
+    <t>Threshold</t>
   </si>
 </sst>
 </file>
@@ -127,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -143,6 +159,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,7 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
@@ -548,10 +565,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -562,7 +579,7 @@
     <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -575,8 +592,14 @@
       <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -584,13 +607,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="5">
-        <v>100</v>
+        <f>MAX(ecological_params!B2:D2)</f>
+        <v>83.6</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -598,13 +624,16 @@
         <v>0</v>
       </c>
       <c r="C3" s="5">
-        <v>100</v>
+        <f>MAX(ecological_params!B3:D3)</f>
+        <v>55.6</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -612,11 +641,14 @@
         <v>0</v>
       </c>
       <c r="C4" s="5">
-        <v>100</v>
+        <f>MAX(ecological_params!B4:D4)</f>
+        <v>65.8</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
       </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>